<commit_message>
Recalculated heat transfer to the air using BMT
</commit_message>
<xml_diff>
--- a/Forced Convection/Forced Convection Calculations.xlsx
+++ b/Forced Convection/Forced Convection Calculations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Experiment</t>
   </si>
@@ -58,7 +58,13 @@
     <t>Heat Loss</t>
   </si>
   <si>
-    <t>Heat Transfer</t>
+    <t>Heat Transfer (q_gen - q_loss)</t>
+  </si>
+  <si>
+    <t>Bulk Mean Temperature</t>
+  </si>
+  <si>
+    <t>Heat Transfer (BMT)</t>
   </si>
   <si>
     <t>Test 1 - High MFR Low Current</t>
@@ -428,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -442,10 +448,13 @@
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="9" max="10" width="18.7109375" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" customWidth="1"/>
-    <col min="12" max="15" width="18.7109375" customWidth="1"/>
+    <col min="12" max="14" width="18.7109375" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" customWidth="1"/>
+    <col min="16" max="16" width="21.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,10 +500,16 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>0.5702300006</v>
@@ -538,10 +553,16 @@
       <c r="O2">
         <v>752.247010782621</v>
       </c>
+      <c r="P2">
+        <v>1.944074140543679</v>
+      </c>
+      <c r="Q2">
+        <v>1424.052505355127</v>
+      </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>0.5664200006</v>
@@ -585,10 +606,16 @@
       <c r="O3">
         <v>1769.96515163397</v>
       </c>
+      <c r="P3">
+        <v>5.020557813103682</v>
+      </c>
+      <c r="Q3">
+        <v>3665.178925903648</v>
+      </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>0.3098800003</v>
@@ -632,10 +659,16 @@
       <c r="O4">
         <v>1672.29956730686</v>
       </c>
+      <c r="P4">
+        <v>6.721114306937997</v>
+      </c>
+      <c r="Q4">
+        <v>3577.242197580631</v>
+      </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>0.3136900003</v>
@@ -678,6 +711,12 @@
       </c>
       <c r="O5">
         <v>624.2975017411634</v>
+      </c>
+      <c r="P5">
+        <v>2.920085621750038</v>
+      </c>
+      <c r="Q5">
+        <v>1562.348859539467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Predicted and plotted the air temperature distribution
</commit_message>
<xml_diff>
--- a/Forced Convection/Forced Convection Calculations.xlsx
+++ b/Forced Convection/Forced Convection Calculations.xlsx
@@ -61,22 +61,22 @@
     <t>Heat Transfer (q_gen - q_loss)</t>
   </si>
   <si>
-    <t>Bulk Mean Temperature</t>
+    <t>Bulk Mean Temperature Slope</t>
   </si>
   <si>
     <t>Heat Transfer (BMT)</t>
   </si>
   <si>
-    <t>Test 1 - High MFR Low Current</t>
-  </si>
-  <si>
-    <t>Test 2 - High MFR High Current</t>
-  </si>
-  <si>
-    <t>Test 3 - Low MFR High Current</t>
-  </si>
-  <si>
-    <t>Test 4 - Low MFR Low Current</t>
+    <t>Test 1 - High MFR Low Crnt</t>
+  </si>
+  <si>
+    <t>Test 2 - High MFR High Crnt</t>
+  </si>
+  <si>
+    <t>Test 3 - Low MFR High Crnt</t>
+  </si>
+  <si>
+    <t>Test 4 - Low MFR Low Crnt</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="6" width="7.7109375" customWidth="1"/>
@@ -450,7 +450,7 @@
     <col min="11" max="11" width="19.7109375" customWidth="1"/>
     <col min="12" max="14" width="18.7109375" customWidth="1"/>
     <col min="15" max="15" width="30.7109375" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" customWidth="1"/>
+    <col min="16" max="16" width="27.7109375" customWidth="1"/>
     <col min="17" max="17" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -527,19 +527,19 @@
         <v>106</v>
       </c>
       <c r="G2">
-        <v>310.5</v>
+        <v>310.65</v>
       </c>
       <c r="H2">
-        <v>325</v>
+        <v>325.15</v>
       </c>
       <c r="I2">
         <v>106906.4817833239</v>
       </c>
       <c r="J2">
-        <v>1.199424120412052</v>
+        <v>1.198844968253475</v>
       </c>
       <c r="K2">
-        <v>0.07437426451006425</v>
+        <v>0.07435630621823901</v>
       </c>
       <c r="L2">
         <v>222.6</v>
@@ -557,7 +557,7 @@
         <v>1.944074140543679</v>
       </c>
       <c r="Q2">
-        <v>1424.052505355127</v>
+        <v>1423.708655898139</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -580,19 +580,19 @@
         <v>161</v>
       </c>
       <c r="G3">
-        <v>312.5</v>
+        <v>312.65</v>
       </c>
       <c r="H3">
-        <v>340</v>
+        <v>340.15</v>
       </c>
       <c r="I3">
         <v>106869.1890320269</v>
       </c>
       <c r="J3">
-        <v>1.19133208237529</v>
+        <v>1.190760517326973</v>
       </c>
       <c r="K3">
-        <v>0.07412295311043976</v>
+        <v>0.07410517000335579</v>
       </c>
       <c r="L3">
         <v>483</v>
@@ -610,7 +610,7 @@
         <v>5.020557813103682</v>
       </c>
       <c r="Q3">
-        <v>3665.178925903648</v>
+        <v>3664.299599506274</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -633,19 +633,19 @@
         <v>160</v>
       </c>
       <c r="G4">
-        <v>313.8</v>
+        <v>313.95</v>
       </c>
       <c r="H4">
-        <v>347</v>
+        <v>347.15</v>
       </c>
       <c r="I4">
         <v>104358.1437750924</v>
       </c>
       <c r="J4">
-        <v>1.158520576558349</v>
+        <v>1.157967055021532</v>
       </c>
       <c r="K4">
-        <v>0.05404015285743295</v>
+        <v>0.05402724157953815</v>
       </c>
       <c r="L4">
         <v>480</v>
@@ -663,7 +663,7 @@
         <v>6.721114306937997</v>
       </c>
       <c r="Q4">
-        <v>3577.242197580631</v>
+        <v>3576.387522571998</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -686,19 +686,19 @@
         <v>105</v>
       </c>
       <c r="G5">
-        <v>314.17</v>
+        <v>314.32</v>
       </c>
       <c r="H5">
-        <v>332</v>
+        <v>332.15</v>
       </c>
       <c r="I5">
         <v>104395.4365263894</v>
       </c>
       <c r="J5">
-        <v>1.157569693381526</v>
+        <v>1.15701727720054</v>
       </c>
       <c r="K5">
-        <v>0.05432402421356729</v>
+        <v>0.05431106039320174</v>
       </c>
       <c r="L5">
         <v>210</v>
@@ -716,7 +716,7 @@
         <v>2.920085621750038</v>
       </c>
       <c r="Q5">
-        <v>1562.348859539467</v>
+        <v>1561.97602247048</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed heat transfer coefficient calculation
That went much smoother than expected
</commit_message>
<xml_diff>
--- a/Forced Convection/Forced Convection Calculations.xlsx
+++ b/Forced Convection/Forced Convection Calculations.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/939c1b26bea70f0b/Personal/GitHub/School-Programs/Forced Convection/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_BC0DB2BBE91D0437C264B4CDBCB4D9A87452F02D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Experiment</t>
   </si>
@@ -65,6 +71,9 @@
   </si>
   <si>
     <t>Heat Transfer (BMT)</t>
+  </si>
+  <si>
+    <t>Heat Transfer Coefficient</t>
   </si>
   <si>
     <t>Test 1 - High MFR Low Crnt</t>
@@ -82,8 +91,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,13 +155,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -190,7 +207,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -224,6 +241,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -258,9 +276,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -433,28 +452,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="10" width="18.7109375" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" customWidth="1"/>
-    <col min="12" max="14" width="18.7109375" customWidth="1"/>
-    <col min="15" max="15" width="30.7109375" customWidth="1"/>
-    <col min="16" max="16" width="27.7109375" customWidth="1"/>
-    <col min="17" max="17" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="6" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="10" width="18.6640625" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
+    <col min="12" max="14" width="18.6640625" customWidth="1"/>
+    <col min="15" max="15" width="30.6640625" customWidth="1"/>
+    <col min="16" max="16" width="27.6640625" customWidth="1"/>
+    <col min="17" max="17" width="19.6640625" customWidth="1"/>
+    <col min="18" max="18" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,16 +526,19 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2">
-        <v>0.5702300006</v>
+        <v>0.57023000059999995</v>
       </c>
       <c r="C2">
-        <v>0.1612900002</v>
+        <v>0.16129000020000001</v>
       </c>
       <c r="D2">
         <v>0.1054100001</v>
@@ -527,19 +550,19 @@
         <v>106</v>
       </c>
       <c r="G2">
-        <v>310.65</v>
+        <v>310.64999999999998</v>
       </c>
       <c r="H2">
-        <v>325.15</v>
+        <v>325.14999999999998</v>
       </c>
       <c r="I2">
-        <v>106906.4817833239</v>
+        <v>106906.48178332391</v>
       </c>
       <c r="J2">
         <v>1.198844968253475</v>
       </c>
       <c r="K2">
-        <v>0.07435630621823901</v>
+        <v>7.4356306218239007E-2</v>
       </c>
       <c r="L2">
         <v>222.6</v>
@@ -548,30 +571,33 @@
         <v>1239.771593117234</v>
       </c>
       <c r="N2">
-        <v>487.5245823346135</v>
+        <v>487.52458233461351</v>
       </c>
       <c r="O2">
-        <v>752.247010782621</v>
+        <v>752.24701078262103</v>
       </c>
       <c r="P2">
         <v>1.944074140543679</v>
       </c>
       <c r="Q2">
-        <v>1423.708655898139</v>
+        <v>1423.7086558981391</v>
+      </c>
+      <c r="R2">
+        <v>93.367340989409044</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3">
-        <v>0.5664200006</v>
+        <v>0.56642000059999997</v>
       </c>
       <c r="C3">
         <v>0.1574800002</v>
       </c>
       <c r="D3">
-        <v>0.1092200001</v>
+        <v>0.10922000010000001</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -580,7 +606,7 @@
         <v>161</v>
       </c>
       <c r="G3">
-        <v>312.65</v>
+        <v>312.64999999999998</v>
       </c>
       <c r="H3">
         <v>340.15</v>
@@ -589,42 +615,45 @@
         <v>106869.1890320269</v>
       </c>
       <c r="J3">
-        <v>1.190760517326973</v>
+        <v>1.1907605173269731</v>
       </c>
       <c r="K3">
-        <v>0.07410517000335579</v>
+        <v>7.4105170003355786E-2</v>
       </c>
       <c r="L3">
         <v>483</v>
       </c>
       <c r="M3">
-        <v>2690.070437895886</v>
+        <v>2690.0704378958858</v>
       </c>
       <c r="N3">
-        <v>920.1052862619158</v>
+        <v>920.10528626191581</v>
       </c>
       <c r="O3">
         <v>1769.96515163397</v>
       </c>
       <c r="P3">
-        <v>5.020557813103682</v>
+        <v>5.0205578131036823</v>
       </c>
       <c r="Q3">
-        <v>3664.299599506274</v>
+        <v>3664.2995995062738</v>
+      </c>
+      <c r="R3">
+        <v>112.42574902742849</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>0.3098800003</v>
+        <v>0.30988000030000001</v>
       </c>
       <c r="C4">
-        <v>0.08636000009</v>
+        <v>8.636000009E-2</v>
       </c>
       <c r="D4">
-        <v>0.06604000006999999</v>
+        <v>6.6040000069999993E-2</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -639,45 +668,48 @@
         <v>347.15</v>
       </c>
       <c r="I4">
-        <v>104358.1437750924</v>
+        <v>104358.14377509239</v>
       </c>
       <c r="J4">
         <v>1.157967055021532</v>
       </c>
       <c r="K4">
-        <v>0.05402724157953815</v>
+        <v>5.402724157953815E-2</v>
       </c>
       <c r="L4">
         <v>480</v>
       </c>
       <c r="M4">
-        <v>2673.361925859265</v>
+        <v>2673.3619258592648</v>
       </c>
       <c r="N4">
         <v>1001.062358552405</v>
       </c>
       <c r="O4">
-        <v>1672.29956730686</v>
+        <v>1672.2995673068599</v>
       </c>
       <c r="P4">
-        <v>6.721114306937997</v>
+        <v>6.7211143069379968</v>
       </c>
       <c r="Q4">
         <v>3576.387522571998</v>
       </c>
+      <c r="R4">
+        <v>82.643192133033367</v>
+      </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5">
-        <v>0.3136900003</v>
+        <v>0.31369000029999999</v>
       </c>
       <c r="C5">
-        <v>0.08763000008999999</v>
+        <v>8.7630000089999993E-2</v>
       </c>
       <c r="D5">
-        <v>0.06299200006</v>
+        <v>6.2992000059999997E-2</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -698,7 +730,7 @@
         <v>1.15701727720054</v>
       </c>
       <c r="K5">
-        <v>0.05431106039320174</v>
+        <v>5.4311060393201743E-2</v>
       </c>
       <c r="L5">
         <v>210</v>
@@ -707,16 +739,19 @@
         <v>1169.595842563429</v>
       </c>
       <c r="N5">
-        <v>545.2983408222651</v>
+        <v>545.29834082226512</v>
       </c>
       <c r="O5">
-        <v>624.2975017411634</v>
+        <v>624.29750174116339</v>
       </c>
       <c r="P5">
-        <v>2.920085621750038</v>
+        <v>2.9200856217500379</v>
       </c>
       <c r="Q5">
-        <v>1561.97602247048</v>
+        <v>1561.9760224704801</v>
+      </c>
+      <c r="R5">
+        <v>65.742888212295099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reynolds number and two calculations for nusselt number
Created a new branch to twork on this, checkouted the main branch and forgot
</commit_message>
<xml_diff>
--- a/Forced Convection/Forced Convection Calculations.xlsx
+++ b/Forced Convection/Forced Convection Calculations.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/939c1b26bea70f0b/Personal/GitHub/School-Programs/Forced Convection/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_BC0DB2BBE91D0437C264B4CDBCB4D9A87452F02D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Experiment</t>
   </si>
@@ -74,6 +68,15 @@
   </si>
   <si>
     <t>Heat Transfer Coefficient</t>
+  </si>
+  <si>
+    <t>Reynolds Number</t>
+  </si>
+  <si>
+    <t>Theoretical Nu</t>
+  </si>
+  <si>
+    <t>Correlated Nu</t>
   </si>
   <si>
     <t>Test 1 - High MFR Low Crnt</t>
@@ -91,8 +94,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,21 +158,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -207,7 +202,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -241,7 +236,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -276,10 +270,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -452,29 +445,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="6" width="7.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="10" width="18.6640625" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" customWidth="1"/>
-    <col min="12" max="14" width="18.6640625" customWidth="1"/>
-    <col min="15" max="15" width="30.6640625" customWidth="1"/>
-    <col min="16" max="16" width="27.6640625" customWidth="1"/>
-    <col min="17" max="17" width="19.6640625" customWidth="1"/>
-    <col min="18" max="18" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+    <col min="12" max="14" width="18.7109375" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" customWidth="1"/>
+    <col min="16" max="16" width="27.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" customWidth="1"/>
+    <col min="18" max="18" width="25.7109375" customWidth="1"/>
+    <col min="19" max="21" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -529,16 +523,25 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2">
-        <v>0.57023000059999995</v>
+        <v>0.5702300006</v>
       </c>
       <c r="C2">
-        <v>0.16129000020000001</v>
+        <v>0.1612900002</v>
       </c>
       <c r="D2">
         <v>0.1054100001</v>
@@ -550,19 +553,19 @@
         <v>106</v>
       </c>
       <c r="G2">
-        <v>310.64999999999998</v>
+        <v>310.65</v>
       </c>
       <c r="H2">
-        <v>325.14999999999998</v>
+        <v>325.15</v>
       </c>
       <c r="I2">
-        <v>106906.48178332391</v>
+        <v>106906.4817833239</v>
       </c>
       <c r="J2">
         <v>1.198844968253475</v>
       </c>
       <c r="K2">
-        <v>7.4356306218239007E-2</v>
+        <v>0.07435630621823901</v>
       </c>
       <c r="L2">
         <v>222.6</v>
@@ -571,33 +574,42 @@
         <v>1239.771593117234</v>
       </c>
       <c r="N2">
-        <v>487.52458233461351</v>
+        <v>487.5245823346135</v>
       </c>
       <c r="O2">
-        <v>752.24701078262103</v>
+        <v>752.247010782621</v>
       </c>
       <c r="P2">
         <v>1.944074140543679</v>
       </c>
       <c r="Q2">
-        <v>1423.7086558981391</v>
+        <v>1423.708655898139</v>
       </c>
       <c r="R2">
-        <v>93.367340989409044</v>
+        <v>93.36734098940904</v>
+      </c>
+      <c r="S2">
+        <v>157269.8347380281</v>
+      </c>
+      <c r="T2">
+        <v>108.7396067737367</v>
+      </c>
+      <c r="U2">
+        <v>287.6152740362283</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>0.56642000059999997</v>
+        <v>0.5664200006</v>
       </c>
       <c r="C3">
         <v>0.1574800002</v>
       </c>
       <c r="D3">
-        <v>0.10922000010000001</v>
+        <v>0.1092200001</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -606,7 +618,7 @@
         <v>161</v>
       </c>
       <c r="G3">
-        <v>312.64999999999998</v>
+        <v>312.65</v>
       </c>
       <c r="H3">
         <v>340.15</v>
@@ -615,45 +627,54 @@
         <v>106869.1890320269</v>
       </c>
       <c r="J3">
-        <v>1.1907605173269731</v>
+        <v>1.190760517326973</v>
       </c>
       <c r="K3">
-        <v>7.4105170003355786E-2</v>
+        <v>0.07410517000335579</v>
       </c>
       <c r="L3">
         <v>483</v>
       </c>
       <c r="M3">
-        <v>2690.0704378958858</v>
+        <v>2690.070437895886</v>
       </c>
       <c r="N3">
-        <v>920.10528626191581</v>
+        <v>920.1052862619158</v>
       </c>
       <c r="O3">
         <v>1769.96515163397</v>
       </c>
       <c r="P3">
-        <v>5.0205578131036823</v>
+        <v>5.020557813103682</v>
       </c>
       <c r="Q3">
-        <v>3664.2995995062738</v>
+        <v>3664.299599506274</v>
       </c>
       <c r="R3">
-        <v>112.42574902742849</v>
+        <v>112.4257490274285</v>
+      </c>
+      <c r="S3">
+        <v>156738.6605442012</v>
+      </c>
+      <c r="T3">
+        <v>130.9358455637301</v>
+      </c>
+      <c r="U3">
+        <v>286.8378815740913</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4">
-        <v>0.30988000030000001</v>
+        <v>0.3098800003</v>
       </c>
       <c r="C4">
-        <v>8.636000009E-2</v>
+        <v>0.08636000009</v>
       </c>
       <c r="D4">
-        <v>6.6040000069999993E-2</v>
+        <v>0.06604000006999999</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -668,48 +689,57 @@
         <v>347.15</v>
       </c>
       <c r="I4">
-        <v>104358.14377509239</v>
+        <v>104358.1437750924</v>
       </c>
       <c r="J4">
         <v>1.157967055021532</v>
       </c>
       <c r="K4">
-        <v>5.402724157953815E-2</v>
+        <v>0.05402724157953815</v>
       </c>
       <c r="L4">
         <v>480</v>
       </c>
       <c r="M4">
-        <v>2673.3619258592648</v>
+        <v>2673.361925859265</v>
       </c>
       <c r="N4">
         <v>1001.062358552405</v>
       </c>
       <c r="O4">
-        <v>1672.2995673068599</v>
+        <v>1672.29956730686</v>
       </c>
       <c r="P4">
-        <v>6.7211143069379968</v>
+        <v>6.721114306937997</v>
       </c>
       <c r="Q4">
         <v>3576.387522571998</v>
       </c>
       <c r="R4">
-        <v>82.643192133033367</v>
+        <v>82.64319213303337</v>
+      </c>
+      <c r="S4">
+        <v>114272.1550694953</v>
+      </c>
+      <c r="T4">
+        <v>96.24980340922207</v>
+      </c>
+      <c r="U4">
+        <v>222.765501999959</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B5">
-        <v>0.31369000029999999</v>
+        <v>0.3136900003</v>
       </c>
       <c r="C5">
-        <v>8.7630000089999993E-2</v>
+        <v>0.08763000008999999</v>
       </c>
       <c r="D5">
-        <v>6.2992000059999997E-2</v>
+        <v>0.06299200006</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -730,7 +760,7 @@
         <v>1.15701727720054</v>
       </c>
       <c r="K5">
-        <v>5.4311060393201743E-2</v>
+        <v>0.05431106039320174</v>
       </c>
       <c r="L5">
         <v>210</v>
@@ -739,19 +769,28 @@
         <v>1169.595842563429</v>
       </c>
       <c r="N5">
-        <v>545.29834082226512</v>
+        <v>545.2983408222651</v>
       </c>
       <c r="O5">
-        <v>624.29750174116339</v>
+        <v>624.2975017411634</v>
       </c>
       <c r="P5">
-        <v>2.9200856217500379</v>
+        <v>2.920085621750038</v>
       </c>
       <c r="Q5">
-        <v>1561.9760224704801</v>
+        <v>1561.97602247048</v>
       </c>
       <c r="R5">
-        <v>65.742888212295099</v>
+        <v>65.7428882122951</v>
+      </c>
+      <c r="S5">
+        <v>114872.4557055894</v>
+      </c>
+      <c r="T5">
+        <v>76.56698516439083</v>
+      </c>
+      <c r="U5">
+        <v>223.7012062043979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed theoretical and correlated calculations for f
</commit_message>
<xml_diff>
--- a/Forced Convection/Forced Convection Calculations.xlsx
+++ b/Forced Convection/Forced Convection Calculations.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/939c1b26bea70f0b/Personal/GitHub/School-Programs/Forced Convection/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_85C593A5E91D04C7C85CA8B354F1F7567552B741" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Experiment</t>
   </si>
@@ -77,6 +83,12 @@
   </si>
   <si>
     <t>Correlated Nu</t>
+  </si>
+  <si>
+    <t>Theoretical Friction Factor</t>
+  </si>
+  <si>
+    <t>Correlated Friction Factor</t>
   </si>
   <si>
     <t>Test 1 - High MFR Low Crnt</t>
@@ -94,8 +106,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,13 +170,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -202,7 +222,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -236,6 +256,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -270,9 +291,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -445,30 +467,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="10" width="18.7109375" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" customWidth="1"/>
-    <col min="12" max="14" width="18.7109375" customWidth="1"/>
-    <col min="15" max="15" width="30.7109375" customWidth="1"/>
-    <col min="16" max="16" width="27.7109375" customWidth="1"/>
-    <col min="17" max="17" width="19.7109375" customWidth="1"/>
-    <col min="18" max="18" width="25.7109375" customWidth="1"/>
-    <col min="19" max="21" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="6" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="10" width="18.6640625" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
+    <col min="12" max="14" width="18.6640625" customWidth="1"/>
+    <col min="15" max="15" width="30.6640625" customWidth="1"/>
+    <col min="16" max="16" width="27.6640625" customWidth="1"/>
+    <col min="17" max="17" width="19.6640625" customWidth="1"/>
+    <col min="18" max="18" width="25.6640625" customWidth="1"/>
+    <col min="19" max="21" width="18.6640625" customWidth="1"/>
+    <col min="22" max="22" width="27.6640625" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,16 +558,22 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2">
-        <v>0.5702300006</v>
+        <v>0.57023000059999995</v>
       </c>
       <c r="C2">
-        <v>0.1612900002</v>
+        <v>0.16129000020000001</v>
       </c>
       <c r="D2">
         <v>0.1054100001</v>
@@ -553,19 +585,19 @@
         <v>106</v>
       </c>
       <c r="G2">
-        <v>310.65</v>
+        <v>310.64999999999998</v>
       </c>
       <c r="H2">
-        <v>325.15</v>
+        <v>325.14999999999998</v>
       </c>
       <c r="I2">
-        <v>106906.4817833239</v>
+        <v>106906.48178332391</v>
       </c>
       <c r="J2">
         <v>1.198844968253475</v>
       </c>
       <c r="K2">
-        <v>0.07435630621823901</v>
+        <v>7.4356306218239007E-2</v>
       </c>
       <c r="L2">
         <v>222.6</v>
@@ -574,22 +606,22 @@
         <v>1239.771593117234</v>
       </c>
       <c r="N2">
-        <v>487.5245823346135</v>
+        <v>487.52458233461351</v>
       </c>
       <c r="O2">
-        <v>752.247010782621</v>
+        <v>752.24701078262103</v>
       </c>
       <c r="P2">
         <v>1.944074140543679</v>
       </c>
       <c r="Q2">
-        <v>1423.708655898139</v>
+        <v>1423.7086558981391</v>
       </c>
       <c r="R2">
-        <v>93.36734098940904</v>
+        <v>93.367340989409044</v>
       </c>
       <c r="S2">
-        <v>157269.8347380281</v>
+        <v>157269.83473802809</v>
       </c>
       <c r="T2">
         <v>108.7396067737367</v>
@@ -597,19 +629,25 @@
       <c r="U2">
         <v>287.6152740362283</v>
       </c>
+      <c r="V2">
+        <v>5.8075053463555138E-3</v>
+      </c>
+      <c r="W2">
+        <v>1.5868129094924681E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3">
-        <v>0.5664200006</v>
+        <v>0.56642000059999997</v>
       </c>
       <c r="C3">
         <v>0.1574800002</v>
       </c>
       <c r="D3">
-        <v>0.1092200001</v>
+        <v>0.10922000010000001</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -618,7 +656,7 @@
         <v>161</v>
       </c>
       <c r="G3">
-        <v>312.65</v>
+        <v>312.64999999999998</v>
       </c>
       <c r="H3">
         <v>340.15</v>
@@ -627,54 +665,60 @@
         <v>106869.1890320269</v>
       </c>
       <c r="J3">
-        <v>1.190760517326973</v>
+        <v>1.1907605173269731</v>
       </c>
       <c r="K3">
-        <v>0.07410517000335579</v>
+        <v>7.4105170003355786E-2</v>
       </c>
       <c r="L3">
         <v>483</v>
       </c>
       <c r="M3">
-        <v>2690.070437895886</v>
+        <v>2690.0704378958858</v>
       </c>
       <c r="N3">
-        <v>920.1052862619158</v>
+        <v>920.10528626191581</v>
       </c>
       <c r="O3">
         <v>1769.96515163397</v>
       </c>
       <c r="P3">
-        <v>5.020557813103682</v>
+        <v>5.0205578131036823</v>
       </c>
       <c r="Q3">
-        <v>3664.299599506274</v>
+        <v>3664.2995995062738</v>
       </c>
       <c r="R3">
-        <v>112.4257490274285</v>
+        <v>112.42574902742849</v>
       </c>
       <c r="S3">
-        <v>156738.6605442012</v>
+        <v>156738.66054420121</v>
       </c>
       <c r="T3">
-        <v>130.9358455637301</v>
+        <v>130.93584556373011</v>
       </c>
       <c r="U3">
-        <v>286.8378815740913</v>
+        <v>286.83788157409128</v>
+      </c>
+      <c r="V3">
+        <v>6.0174151779523602E-3</v>
+      </c>
+      <c r="W3">
+        <v>1.5881555983615441E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4">
-        <v>0.3098800003</v>
+        <v>0.30988000030000001</v>
       </c>
       <c r="C4">
-        <v>0.08636000009</v>
+        <v>8.636000009E-2</v>
       </c>
       <c r="D4">
-        <v>0.06604000006999999</v>
+        <v>6.6040000069999993E-2</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -689,57 +733,63 @@
         <v>347.15</v>
       </c>
       <c r="I4">
-        <v>104358.1437750924</v>
+        <v>104358.14377509239</v>
       </c>
       <c r="J4">
         <v>1.157967055021532</v>
       </c>
       <c r="K4">
-        <v>0.05402724157953815</v>
+        <v>5.402724157953815E-2</v>
       </c>
       <c r="L4">
         <v>480</v>
       </c>
       <c r="M4">
-        <v>2673.361925859265</v>
+        <v>2673.3619258592648</v>
       </c>
       <c r="N4">
         <v>1001.062358552405</v>
       </c>
       <c r="O4">
-        <v>1672.29956730686</v>
+        <v>1672.2995673068599</v>
       </c>
       <c r="P4">
-        <v>6.721114306937997</v>
+        <v>6.7211143069379968</v>
       </c>
       <c r="Q4">
         <v>3576.387522571998</v>
       </c>
       <c r="R4">
-        <v>82.64319213303337</v>
+        <v>82.643192133033367</v>
       </c>
       <c r="S4">
         <v>114272.1550694953</v>
       </c>
       <c r="T4">
-        <v>96.24980340922207</v>
+        <v>96.249803409222068</v>
       </c>
       <c r="U4">
-        <v>222.765501999959</v>
+        <v>222.76550199995901</v>
+      </c>
+      <c r="V4">
+        <v>6.6566860305280863E-3</v>
+      </c>
+      <c r="W4">
+        <v>1.7187075238643029E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5">
-        <v>0.3136900003</v>
+        <v>0.31369000029999999</v>
       </c>
       <c r="C5">
-        <v>0.08763000008999999</v>
+        <v>8.7630000089999993E-2</v>
       </c>
       <c r="D5">
-        <v>0.06299200006</v>
+        <v>6.2992000059999997E-2</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -760,7 +810,7 @@
         <v>1.15701727720054</v>
       </c>
       <c r="K5">
-        <v>0.05431106039320174</v>
+        <v>5.4311060393201743E-2</v>
       </c>
       <c r="L5">
         <v>210</v>
@@ -769,28 +819,34 @@
         <v>1169.595842563429</v>
       </c>
       <c r="N5">
-        <v>545.2983408222651</v>
+        <v>545.29834082226512</v>
       </c>
       <c r="O5">
-        <v>624.2975017411634</v>
+        <v>624.29750174116339</v>
       </c>
       <c r="P5">
-        <v>2.920085621750038</v>
+        <v>2.9200856217500379</v>
       </c>
       <c r="Q5">
-        <v>1561.97602247048</v>
+        <v>1561.9760224704801</v>
       </c>
       <c r="R5">
-        <v>65.7428882122951</v>
+        <v>65.742888212295099</v>
       </c>
       <c r="S5">
         <v>114872.4557055894</v>
       </c>
       <c r="T5">
-        <v>76.56698516439083</v>
+        <v>76.566985164390829</v>
       </c>
       <c r="U5">
-        <v>223.7012062043979</v>
+        <v>223.70120620439789</v>
+      </c>
+      <c r="V5">
+        <v>6.2781121830668557E-3</v>
+      </c>
+      <c r="W5">
+        <v>1.7164577041029389E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed theoretical and correlated calculations for Stanton number
</commit_message>
<xml_diff>
--- a/Forced Convection/Forced Convection Calculations.xlsx
+++ b/Forced Convection/Forced Convection Calculations.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/939c1b26bea70f0b/Personal/GitHub/School-Programs/Forced Convection/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_85C593A5E91D04C7C85CA8B354F1F7567552B741" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Experiment</t>
   </si>
@@ -89,6 +83,12 @@
   </si>
   <si>
     <t>Correlated Friction Factor</t>
+  </si>
+  <si>
+    <t>Theoretical Stanton Number</t>
+  </si>
+  <si>
+    <t>Correlated Stanton Number</t>
   </si>
   <si>
     <t>Test 1 - High MFR Low Crnt</t>
@@ -106,8 +106,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,21 +170,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -222,7 +214,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -256,7 +248,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -291,10 +282,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -467,34 +457,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="6" width="7.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="10" width="18.6640625" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" customWidth="1"/>
-    <col min="12" max="14" width="18.6640625" customWidth="1"/>
-    <col min="15" max="15" width="30.6640625" customWidth="1"/>
-    <col min="16" max="16" width="27.6640625" customWidth="1"/>
-    <col min="17" max="17" width="19.6640625" customWidth="1"/>
-    <col min="18" max="18" width="25.6640625" customWidth="1"/>
-    <col min="19" max="21" width="18.6640625" customWidth="1"/>
-    <col min="22" max="22" width="27.6640625" customWidth="1"/>
-    <col min="23" max="23" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+    <col min="12" max="14" width="18.7109375" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" customWidth="1"/>
+    <col min="16" max="16" width="27.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" customWidth="1"/>
+    <col min="18" max="18" width="25.7109375" customWidth="1"/>
+    <col min="19" max="21" width="18.7109375" customWidth="1"/>
+    <col min="22" max="22" width="27.7109375" customWidth="1"/>
+    <col min="23" max="24" width="26.7109375" customWidth="1"/>
+    <col min="25" max="25" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,16 +553,22 @@
       <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>0.57023000059999995</v>
+        <v>0.5702300006</v>
       </c>
       <c r="C2">
-        <v>0.16129000020000001</v>
+        <v>0.1612900002</v>
       </c>
       <c r="D2">
         <v>0.1054100001</v>
@@ -585,19 +580,19 @@
         <v>106</v>
       </c>
       <c r="G2">
-        <v>310.64999999999998</v>
+        <v>310.65</v>
       </c>
       <c r="H2">
-        <v>325.14999999999998</v>
+        <v>325.15</v>
       </c>
       <c r="I2">
-        <v>106906.48178332391</v>
+        <v>106906.4817833239</v>
       </c>
       <c r="J2">
         <v>1.198844968253475</v>
       </c>
       <c r="K2">
-        <v>7.4356306218239007E-2</v>
+        <v>0.07435630621823901</v>
       </c>
       <c r="L2">
         <v>222.6</v>
@@ -606,22 +601,22 @@
         <v>1239.771593117234</v>
       </c>
       <c r="N2">
-        <v>487.52458233461351</v>
+        <v>487.5245823346135</v>
       </c>
       <c r="O2">
-        <v>752.24701078262103</v>
+        <v>752.247010782621</v>
       </c>
       <c r="P2">
         <v>1.944074140543679</v>
       </c>
       <c r="Q2">
-        <v>1423.7086558981391</v>
+        <v>1423.708655898139</v>
       </c>
       <c r="R2">
-        <v>93.367340989409044</v>
+        <v>93.36734098940904</v>
       </c>
       <c r="S2">
-        <v>157269.83473802809</v>
+        <v>157269.8347380281</v>
       </c>
       <c r="T2">
         <v>108.7396067737367</v>
@@ -630,24 +625,30 @@
         <v>287.6152740362283</v>
       </c>
       <c r="V2">
-        <v>5.8075053463555138E-3</v>
+        <v>0.005807505346355514</v>
       </c>
       <c r="W2">
-        <v>1.5868129094924681E-2</v>
+        <v>0.01586812909492468</v>
+      </c>
+      <c r="X2">
+        <v>0.003467963058845684</v>
+      </c>
+      <c r="Y2">
+        <v>0.002499325357727647</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>0.56642000059999997</v>
+        <v>0.5664200006</v>
       </c>
       <c r="C3">
         <v>0.1574800002</v>
       </c>
       <c r="D3">
-        <v>0.10922000010000001</v>
+        <v>0.1092200001</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -656,7 +657,7 @@
         <v>161</v>
       </c>
       <c r="G3">
-        <v>312.64999999999998</v>
+        <v>312.65</v>
       </c>
       <c r="H3">
         <v>340.15</v>
@@ -665,60 +666,66 @@
         <v>106869.1890320269</v>
       </c>
       <c r="J3">
-        <v>1.1907605173269731</v>
+        <v>1.190760517326973</v>
       </c>
       <c r="K3">
-        <v>7.4105170003355786E-2</v>
+        <v>0.07410517000335579</v>
       </c>
       <c r="L3">
         <v>483</v>
       </c>
       <c r="M3">
-        <v>2690.0704378958858</v>
+        <v>2690.070437895886</v>
       </c>
       <c r="N3">
-        <v>920.10528626191581</v>
+        <v>920.1052862619158</v>
       </c>
       <c r="O3">
         <v>1769.96515163397</v>
       </c>
       <c r="P3">
-        <v>5.0205578131036823</v>
+        <v>5.020557813103682</v>
       </c>
       <c r="Q3">
-        <v>3664.2995995062738</v>
+        <v>3664.299599506274</v>
       </c>
       <c r="R3">
-        <v>112.42574902742849</v>
+        <v>112.4257490274285</v>
       </c>
       <c r="S3">
-        <v>156738.66054420121</v>
+        <v>156738.6605442012</v>
       </c>
       <c r="T3">
-        <v>130.93584556373011</v>
+        <v>130.9358455637301</v>
       </c>
       <c r="U3">
-        <v>286.83788157409128</v>
+        <v>286.8378815740913</v>
       </c>
       <c r="V3">
-        <v>6.0174151779523602E-3</v>
+        <v>0.00601741517795236</v>
       </c>
       <c r="W3">
-        <v>1.5881555983615441E-2</v>
+        <v>0.01588155598361544</v>
+      </c>
+      <c r="X3">
+        <v>0.004218452465769974</v>
+      </c>
+      <c r="Y3">
+        <v>0.002501440173102507</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B4">
-        <v>0.30988000030000001</v>
+        <v>0.3098800003</v>
       </c>
       <c r="C4">
-        <v>8.636000009E-2</v>
+        <v>0.08636000009</v>
       </c>
       <c r="D4">
-        <v>6.6040000069999993E-2</v>
+        <v>0.06604000006999999</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -733,63 +740,69 @@
         <v>347.15</v>
       </c>
       <c r="I4">
-        <v>104358.14377509239</v>
+        <v>104358.1437750924</v>
       </c>
       <c r="J4">
         <v>1.157967055021532</v>
       </c>
       <c r="K4">
-        <v>5.402724157953815E-2</v>
+        <v>0.05402724157953815</v>
       </c>
       <c r="L4">
         <v>480</v>
       </c>
       <c r="M4">
-        <v>2673.3619258592648</v>
+        <v>2673.361925859265</v>
       </c>
       <c r="N4">
         <v>1001.062358552405</v>
       </c>
       <c r="O4">
-        <v>1672.2995673068599</v>
+        <v>1672.29956730686</v>
       </c>
       <c r="P4">
-        <v>6.7211143069379968</v>
+        <v>6.721114306937997</v>
       </c>
       <c r="Q4">
         <v>3576.387522571998</v>
       </c>
       <c r="R4">
-        <v>82.643192133033367</v>
+        <v>82.64319213303337</v>
       </c>
       <c r="S4">
         <v>114272.1550694953</v>
       </c>
       <c r="T4">
-        <v>96.249803409222068</v>
+        <v>96.24980340922207</v>
       </c>
       <c r="U4">
-        <v>222.76550199995901</v>
+        <v>222.765501999959</v>
       </c>
       <c r="V4">
-        <v>6.6566860305280863E-3</v>
+        <v>0.006656686030528086</v>
       </c>
       <c r="W4">
-        <v>1.7187075238643029E-2</v>
+        <v>0.01718707523864303</v>
+      </c>
+      <c r="X4">
+        <v>0.004373794654161028</v>
+      </c>
+      <c r="Y4">
+        <v>0.002707067273787979</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B5">
-        <v>0.31369000029999999</v>
+        <v>0.3136900003</v>
       </c>
       <c r="C5">
-        <v>8.7630000089999993E-2</v>
+        <v>0.08763000008999999</v>
       </c>
       <c r="D5">
-        <v>6.2992000059999997E-2</v>
+        <v>0.06299200006</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -810,7 +823,7 @@
         <v>1.15701727720054</v>
       </c>
       <c r="K5">
-        <v>5.4311060393201743E-2</v>
+        <v>0.05431106039320174</v>
       </c>
       <c r="L5">
         <v>210</v>
@@ -819,34 +832,40 @@
         <v>1169.595842563429</v>
       </c>
       <c r="N5">
-        <v>545.29834082226512</v>
+        <v>545.2983408222651</v>
       </c>
       <c r="O5">
-        <v>624.29750174116339</v>
+        <v>624.2975017411634</v>
       </c>
       <c r="P5">
-        <v>2.9200856217500379</v>
+        <v>2.920085621750038</v>
       </c>
       <c r="Q5">
-        <v>1561.9760224704801</v>
+        <v>1561.97602247048</v>
       </c>
       <c r="R5">
-        <v>65.742888212295099</v>
+        <v>65.7428882122951</v>
       </c>
       <c r="S5">
         <v>114872.4557055894</v>
       </c>
       <c r="T5">
-        <v>76.566985164390829</v>
+        <v>76.56698516439083</v>
       </c>
       <c r="U5">
-        <v>223.70120620439789</v>
+        <v>223.7012062043979</v>
       </c>
       <c r="V5">
-        <v>6.2781121830668557E-3</v>
+        <v>0.006278112183066856</v>
       </c>
       <c r="W5">
-        <v>1.7164577041029389E-2</v>
+        <v>0.01716457704102939</v>
+      </c>
+      <c r="X5">
+        <v>0.003464024518265738</v>
+      </c>
+      <c r="Y5">
+        <v>0.002703523672934813</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plot the difference between the predicted and measured temperatures
</commit_message>
<xml_diff>
--- a/Forced Convection/Forced Convection Calculations.xlsx
+++ b/Forced Convection/Forced Convection Calculations.xlsx
@@ -625,7 +625,7 @@
         <v>287.6152740362283</v>
       </c>
       <c r="V2">
-        <v>0.005807505346355514</v>
+        <v>0.003078677535596517</v>
       </c>
       <c r="W2">
         <v>0.01586812909492468</v>
@@ -702,7 +702,7 @@
         <v>286.8378815740913</v>
       </c>
       <c r="V3">
-        <v>0.00601741517795236</v>
+        <v>0.002658857872402826</v>
       </c>
       <c r="W3">
         <v>0.01588155598361544</v>
@@ -779,7 +779,7 @@
         <v>222.765501999959</v>
       </c>
       <c r="V4">
-        <v>0.006656686030528086</v>
+        <v>0.002048211086161262</v>
       </c>
       <c r="W4">
         <v>0.01718707523864303</v>
@@ -856,7 +856,7 @@
         <v>223.7012062043979</v>
       </c>
       <c r="V5">
-        <v>0.006278112183066856</v>
+        <v>0.002455551943221542</v>
       </c>
       <c r="W5">
         <v>0.01716457704102939</v>

</xml_diff>